<commit_message>
Add XTRA samples for adding items to Orchestrator queue and sending out emails
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17213" windowHeight="6330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18128" windowHeight="10703"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -83,12 +83,6 @@
     <t>Transactions queue in Orchestrator</t>
   </si>
   <si>
-    <t>Application executable file path</t>
-  </si>
-  <si>
-    <t>Application credentials used to login</t>
-  </si>
-  <si>
     <t>List of workflows to execute for opening applications</t>
   </si>
   <si>
@@ -104,61 +98,115 @@
     <t>InputFile</t>
   </si>
   <si>
-    <t>SampleData.xlsx</t>
-  </si>
-  <si>
     <t>Sample data for running the template</t>
   </si>
   <si>
     <t>ProcessName</t>
   </si>
   <si>
-    <t>Robotic Enterprise Framework</t>
-  </si>
-  <si>
-    <t>ReFrameWork-ChorePile</t>
-  </si>
-  <si>
-    <t>ReFrameWork Template</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notepad/OpenApp, </t>
-  </si>
-  <si>
     <t xml:space="preserve">Notepad/CloseApp, </t>
   </si>
   <si>
     <t>Xtras/EmailTemplate.txt</t>
   </si>
   <si>
-    <t>Template for SendStatusEmail report</t>
-  </si>
-  <si>
     <t>Something meaningful for the user in the given context</t>
   </si>
   <si>
-    <t>ReFrameWork-Credentials</t>
-  </si>
-  <si>
     <t>Exception</t>
   </si>
   <si>
-    <t>OutmailTo</t>
-  </si>
-  <si>
-    <t>OutmailSubject</t>
-  </si>
-  <si>
     <t>Testing ReFrameWork</t>
   </si>
   <si>
-    <t>Recipient for the email report</t>
-  </si>
-  <si>
-    <t>Email report subject line</t>
-  </si>
-  <si>
     <t>love@uipath.com</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Notepad/OpenApp,</t>
+  </si>
+  <si>
+    <t>InputFolder</t>
+  </si>
+  <si>
+    <t>RFW-ChorePile</t>
+  </si>
+  <si>
+    <t>ReFrameWork Performer</t>
+  </si>
+  <si>
+    <t>Robotic Enterprise Framework Template</t>
+  </si>
+  <si>
+    <t>OrchestratorCredential</t>
+  </si>
+  <si>
+    <t>OrchestratorUrl</t>
+  </si>
+  <si>
+    <t>https://demo.uipath.com</t>
+  </si>
+  <si>
+    <t>TestData</t>
+  </si>
+  <si>
+    <t>EmailTo</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t>RFW-SampleLogin</t>
+  </si>
+  <si>
+    <t>RFW-Orchestrator</t>
+  </si>
+  <si>
+    <t>OrchestratorTenant</t>
+  </si>
+  <si>
+    <t>NextJobName</t>
+  </si>
+  <si>
+    <t>XTRAS/SendStatusEmail: Email report subject line</t>
+  </si>
+  <si>
+    <t>XTRAS/SendStatusEmail: Recipient for the email report</t>
+  </si>
+  <si>
+    <t>XTRAS/SendStatusEmail: Template for SendStatusEmail report</t>
+  </si>
+  <si>
+    <t>Orchestrator: Credentials to log into Orchestrator</t>
+  </si>
+  <si>
+    <t>Orchestrator: Tenenacy for public Orchestrator access</t>
+  </si>
+  <si>
+    <t>Orchestrator: Public instance of Orchestrator server</t>
+  </si>
+  <si>
+    <t>Orchestrator: Start an Orchestrator job by its name</t>
+  </si>
+  <si>
+    <t>RFW-Performer</t>
+  </si>
+  <si>
+    <t>Fantastic</t>
+  </si>
+  <si>
+    <t>XTRAS/AddDataToQueue: Input data folder</t>
+  </si>
+  <si>
+    <t>Some application executable file path</t>
+  </si>
+  <si>
+    <t>Some application credentials used to login</t>
+  </si>
+  <si>
+    <t>TestData\Sample1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -558,7 +606,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -581,13 +629,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -607,10 +655,10 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
@@ -618,10 +666,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -632,7 +680,7 @@
         <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -640,10 +688,10 @@
         <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -659,10 +707,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
         <v>17</v>
@@ -670,13 +718,13 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
@@ -684,7 +732,7 @@
         <v>19</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
         <v>20</v>
@@ -703,6 +751,9 @@
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" s="2"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B18" s="2"/>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
@@ -721,7 +772,7 @@
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -736,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -764,7 +815,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -775,7 +826,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -786,15 +837,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="15.1328125" customWidth="1"/>
+    <col min="1" max="1" width="18.9296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.9296875" customWidth="1"/>
     <col min="3" max="3" width="59.6640625" customWidth="1"/>
   </cols>
@@ -810,42 +861,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>45</v>
+      <c r="C11" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId1"/>
+    <hyperlink ref="B11" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Change sample process error rates
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18528"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18128" windowHeight="10703"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18128" windowHeight="10703" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -38,12 +38,6 @@
     <t>EmailTemplate</t>
   </si>
   <si>
-    <t>How many times to retry transactions in case of tehnical issues</t>
-  </si>
-  <si>
-    <t>For technical issues, logging errors and screenshots</t>
-  </si>
-  <si>
     <t>Comments</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>TestData\Sample1.xlsx</t>
+  </si>
+  <si>
+    <t>For system failures, logging screenshots and stack traces</t>
+  </si>
+  <si>
+    <t>How many times to retry transactions in case of issues</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -629,131 +629,125 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" t="s">
-        <v>62</v>
-      </c>
-      <c r="C12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B18" s="2"/>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" s="2"/>
@@ -787,7 +781,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -803,7 +797,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -815,18 +809,18 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -839,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -863,13 +857,13 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
@@ -879,24 +873,24 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
@@ -904,54 +898,54 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B12" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Xtras/OffloadQueue workflow sample for reassembling data into Excel files
</commit_message>
<xml_diff>
--- a/Config.xlsx
+++ b/Config.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -191,9 +191,6 @@
     <t>Fantastic</t>
   </si>
   <si>
-    <t>XTRAS/AddDataToQueue: Input data folder</t>
-  </si>
-  <si>
     <t>Some application executable file path</t>
   </si>
   <si>
@@ -207,6 +204,42 @@
   </si>
   <si>
     <t>How many times to retry transactions in case of issues</t>
+  </si>
+  <si>
+    <t>XTRAS/OnloadQueue: Input data folder</t>
+  </si>
+  <si>
+    <t>OutputPath</t>
+  </si>
+  <si>
+    <t>TestData/Output/[File]</t>
+  </si>
+  <si>
+    <t>XTRAS/OffloadQueue: Output data file path</t>
+  </si>
+  <si>
+    <t>XTRAS/OffloadQueue: Output queue to fetch data from</t>
+  </si>
+  <si>
+    <t>OutputQueue</t>
+  </si>
+  <si>
+    <t>OutputTemplate</t>
+  </si>
+  <si>
+    <t>Xtras/ExcelTemplate.xlsx</t>
+  </si>
+  <si>
+    <t>XTRAS/OffloadQueue: Output Excel template file</t>
+  </si>
+  <si>
+    <t>OutputSheet</t>
+  </si>
+  <si>
+    <t>DataSheet</t>
+  </si>
+  <si>
+    <t>XTRAS/OffloadQueue: Output Excel sheet name</t>
   </si>
 </sst>
 </file>
@@ -680,7 +713,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
@@ -691,7 +724,7 @@
         <v>44</v>
       </c>
       <c r="C8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
@@ -702,7 +735,7 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
@@ -724,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.45">
@@ -743,7 +776,7 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
         <v>24</v>
@@ -831,10 +864,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -863,95 +896,135 @@
         <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="C4"/>
-    </row>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>48</v>
+      <c r="A5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>63</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" t="s">
-        <v>51</v>
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
-      <c r="C10" t="s">
-        <v>52</v>
+      <c r="A10" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B16" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C16" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>47</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B17" t="s">
         <v>55</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C17" t="s">
         <v>54</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-    <hyperlink ref="B11" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1"/>
+    <hyperlink ref="B16" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>